<commit_message>
Added update test results and reports
</commit_message>
<xml_diff>
--- a/meetrapporten/working/metingen.xlsx
+++ b/meetrapporten/working/metingen.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jip\Desktop\Vision_Jip_Tim\meetrapporten\working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jip\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">Meetingen </t>
   </si>
@@ -432,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="O15" sqref="J12:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,9 +446,10 @@
     <col min="5" max="5" width="6.77734375" customWidth="1"/>
     <col min="6" max="6" width="6.109375" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,8 +474,26 @@
       <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J1">
+        <v>1</v>
+      </c>
+      <c r="K1">
+        <v>2</v>
+      </c>
+      <c r="L1">
+        <v>3</v>
+      </c>
+      <c r="M1">
+        <v>4</v>
+      </c>
+      <c r="N1">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -498,10 +517,10 @@
         <v>27622.2</v>
       </c>
       <c r="H2">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -525,35 +544,35 @@
         <v>66503.199999999997</v>
       </c>
       <c r="H3">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -577,10 +596,10 @@
         <v>16408.599999999999</v>
       </c>
       <c r="H11">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -604,10 +623,29 @@
         <v>22135.200000000001</v>
       </c>
       <c r="H12">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="J12">
+        <v>11897.3</v>
+      </c>
+      <c r="K12">
+        <v>11522.7</v>
+      </c>
+      <c r="L12">
+        <v>13794</v>
+      </c>
+      <c r="M12">
+        <v>13949</v>
+      </c>
+      <c r="N12">
+        <v>14138.6</v>
+      </c>
+      <c r="O12">
+        <f>AVERAGE(J12:N12)</f>
+        <v>13060.32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -631,10 +669,29 @@
         <v>22029.599999999999</v>
       </c>
       <c r="H13">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="J13">
+        <v>13026.8</v>
+      </c>
+      <c r="K13">
+        <v>13889.3</v>
+      </c>
+      <c r="L13">
+        <v>13740.1</v>
+      </c>
+      <c r="M13">
+        <v>14030.9</v>
+      </c>
+      <c r="N13">
+        <v>14141</v>
+      </c>
+      <c r="O13">
+        <f>AVERAGE(J13:N13)</f>
+        <v>13765.62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -658,10 +715,29 @@
         <v>17620.400000000001</v>
       </c>
       <c r="H14">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J14">
+        <v>10965.8</v>
+      </c>
+      <c r="K14">
+        <v>13431.8</v>
+      </c>
+      <c r="L14">
+        <v>14317</v>
+      </c>
+      <c r="M14">
+        <v>13389.4</v>
+      </c>
+      <c r="N14">
+        <v>13262.3</v>
+      </c>
+      <c r="O14">
+        <f>AVERAGE(J14:N14)</f>
+        <v>13073.26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -685,7 +761,26 @@
         <v>17452.8</v>
       </c>
       <c r="H15">
-        <v>0.17</v>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J15">
+        <v>11069.8</v>
+      </c>
+      <c r="K15">
+        <v>11589.3</v>
+      </c>
+      <c r="L15">
+        <v>10944</v>
+      </c>
+      <c r="M15">
+        <v>11208</v>
+      </c>
+      <c r="N15">
+        <v>11019.8</v>
+      </c>
+      <c r="O15">
+        <f>AVERAGE(J15:N15)</f>
+        <v>11166.179999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>